<commit_message>
Honestly not sure what the modification is here?
</commit_message>
<xml_diff>
--- a/site_DATAexplore/Laura_AllObs_Abundance.xlsx
+++ b/site_DATAexplore/Laura_AllObs_Abundance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D9A0F5-8119-EA4C-903D-709E237B2CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002FF53C-259C-7540-8D18-2C5A64037D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="28800" windowHeight="15120" xr2:uid="{50156FDB-BF56-F941-9A19-586B72052601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15120" activeTab="1" xr2:uid="{50156FDB-BF56-F941-9A19-586B72052601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="103">
   <si>
     <t>obs_id</t>
   </si>
@@ -333,6 +334,15 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>length_surveyed</t>
+  </si>
+  <si>
+    <t>length_sur</t>
+  </si>
+  <si>
+    <t>length surveyed upstream (km)</t>
   </si>
 </sst>
 </file>
@@ -710,19 +720,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4ED570-FC19-A346-97EB-8C7FB956716A}">
-  <dimension ref="A1:AO52"/>
+  <dimension ref="A1:AP52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,46 +743,49 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -782,47 +795,47 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>40</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>120</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>43.079267999999999</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-123.38822999999999</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>43302</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>40</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -832,47 +845,47 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>15</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>43.080730000000003</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-123.38642</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>43265</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>5</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -882,47 +895,47 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>60</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>43.079389999999997</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>-123.38733000000001</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>43302</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -932,47 +945,47 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>7.5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>43.07161</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-123.37118</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>43354</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>4</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -982,47 +995,47 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>9</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>75</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>43.064118999999998</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>-123.357484</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>43302</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>9</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1032,47 +1045,47 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>30</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>43.063355999999999</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>-123.357287</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>43303</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1082,47 +1095,47 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>200</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>43.062443999999999</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>-123.354012</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>43302</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>4</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1132,47 +1145,47 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>12</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>210</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>43.063693999999998</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-123.352068</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>43302</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>12</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1182,47 +1195,47 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
       <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>0.25</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>43.048726000000002</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>-123.328327</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>43355</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1232,47 +1245,47 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
       <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>43.047269999999997</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>-123.328733</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>43355</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1282,47 +1295,47 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
       <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>20</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>0.25</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>43.046411999999997</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>-123.32916899999999</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>43355</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1332,47 +1345,47 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
       <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>20</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.25</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>43.045456999999999</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>-123.329596</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>43355</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>2</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17">
+    <row r="14" spans="1:17" ht="17">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1382,47 +1395,48 @@
       <c r="C14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
       <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
         <v>0.25</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>42.972178</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>-123.345911</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <v>44061</v>
       </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
       <c r="N14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="17">
+    <row r="15" spans="1:17" ht="17">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1432,47 +1446,48 @@
       <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>2</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <v>42.971291000000001</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>-123.34515399999999</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="6">
+      <c r="M15" s="6">
         <v>44061</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>2</v>
       </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
       <c r="O15" s="4">
         <v>0</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17">
+    <row r="16" spans="1:17" ht="17">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -1482,47 +1497,48 @@
       <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
       <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
         <v>0.25</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <v>42.970297000000002</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>-123.34502000000001</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="6">
+      <c r="M16" s="6">
         <v>44061</v>
       </c>
-      <c r="M16" s="4">
-        <v>1</v>
-      </c>
       <c r="N16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="4">
         <v>0</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="17">
+    <row r="17" spans="1:17" ht="17">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -1532,47 +1548,48 @@
       <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="4">
-        <v>1</v>
-      </c>
       <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
         <v>0.25</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>42.971172000000003</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>-123.34511500000001</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="6">
         <v>44061</v>
       </c>
-      <c r="M17" s="4">
-        <v>1</v>
-      </c>
       <c r="N17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="4">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="17">
+    <row r="18" spans="1:17" ht="17">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -1582,47 +1599,48 @@
       <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>4</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>0.25</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>42.970495</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>-123.344628</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="6">
+      <c r="M18" s="6">
         <v>44061</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>4</v>
       </c>
-      <c r="N18" s="4">
-        <v>0</v>
-      </c>
       <c r="O18" s="4">
         <v>0</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="17">
+    <row r="19" spans="1:17" ht="17">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -1632,47 +1650,48 @@
       <c r="C19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="4">
-        <v>1</v>
-      </c>
       <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
         <v>0.25</v>
       </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
         <v>42.975028000000002</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>-123.34740499999999</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="6">
+      <c r="M19" s="6">
         <v>44062</v>
       </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
       <c r="N19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="17">
+    <row r="20" spans="1:17" ht="17">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
@@ -1682,47 +1701,48 @@
       <c r="C20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
       <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
         <v>0.25</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>42.975099999999998</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <v>-123.347042</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="6">
+      <c r="M20" s="6">
         <v>44062</v>
       </c>
-      <c r="M20" s="4">
-        <v>1</v>
-      </c>
       <c r="N20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="4">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1">
+    <row r="21" spans="1:17" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -1732,47 +1752,48 @@
       <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
       <c r="H21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
         <v>0.25</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>42.973796</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <v>-123.347138</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="6">
+      <c r="M21" s="6">
         <v>44062</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
       <c r="N21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="4">
         <v>0</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="17">
+    <row r="22" spans="1:17" ht="17">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
@@ -1782,47 +1803,47 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
       <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
         <v>0.25</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>42.940215000000002</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>-123.266238</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>44061</v>
       </c>
-      <c r="M22" s="4">
-        <v>0</v>
-      </c>
       <c r="N22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17">
+    <row r="23" spans="1:17" ht="17">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -1832,47 +1853,48 @@
       <c r="C23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>3</v>
       </c>
-      <c r="H23" s="5">
+      <c r="I23" s="5">
         <v>6</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <v>42.940309999999997</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>-123.265443</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="6">
+      <c r="M23" s="6">
         <v>44061</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>2</v>
       </c>
-      <c r="N23" s="4">
-        <v>1</v>
-      </c>
       <c r="O23" s="4">
-        <v>0</v>
-      </c>
-      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17">
+    <row r="24" spans="1:17" ht="17">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -1882,47 +1904,48 @@
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>3</v>
       </c>
-      <c r="H24" s="5">
+      <c r="I24" s="5">
         <v>6</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>42.940340999999997</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>-123.265276</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="L24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L24" s="6">
+      <c r="M24" s="6">
         <v>44061</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>2</v>
       </c>
-      <c r="N24" s="4">
-        <v>1</v>
-      </c>
       <c r="O24" s="4">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="17">
+    <row r="25" spans="1:17" ht="17">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -1932,47 +1955,48 @@
       <c r="C25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="4">
+      <c r="H25" s="4">
         <v>2</v>
       </c>
-      <c r="H25" s="5">
+      <c r="I25" s="5">
         <v>2</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>42.940289999999997</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>-123.265108</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="L25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L25" s="6">
+      <c r="M25" s="6">
         <v>44061</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>2</v>
       </c>
-      <c r="N25" s="4">
-        <v>0</v>
-      </c>
       <c r="O25" s="4">
         <v>0</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="17">
+    <row r="26" spans="1:17" ht="17">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -1982,47 +2006,48 @@
       <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4">
         <v>2</v>
       </c>
-      <c r="H26" s="5">
+      <c r="I26" s="5">
         <v>0.5</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>42.940238999999998</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>-123.26508800000001</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L26" s="6">
+      <c r="M26" s="6">
         <v>44062</v>
       </c>
-      <c r="M26" s="4">
-        <v>0</v>
-      </c>
       <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
         <v>2</v>
       </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="P26" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="34">
+    <row r="27" spans="1:17" ht="34">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -2032,47 +2057,48 @@
       <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G27" s="4">
+      <c r="H27" s="4">
         <v>47</v>
       </c>
-      <c r="H27" s="5">
+      <c r="I27" s="5">
         <v>90</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>42.940491000000002</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>-123.26473</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L27" s="6">
+      <c r="M27" s="6">
         <v>44062</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N27" s="4">
         <v>44</v>
       </c>
-      <c r="N27" s="4">
-        <v>0</v>
-      </c>
       <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
         <v>3</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17">
+    <row r="28" spans="1:17" ht="17">
       <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
@@ -2082,47 +2108,48 @@
       <c r="C28" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D28" s="7"/>
       <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>2</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>10</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>42.959716999999998</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>-123.17582899999999</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L28" s="8">
+      <c r="M28" s="8">
         <v>44047</v>
       </c>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
       <c r="N28" s="4">
         <v>1</v>
       </c>
       <c r="O28" s="4">
-        <v>0</v>
-      </c>
-      <c r="P28" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17">
+    <row r="29" spans="1:17" ht="17">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -2132,47 +2159,47 @@
       <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
       <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
         <v>0.25</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>42.959589000000001</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>-123.176136</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="8">
+      <c r="M29" s="8">
         <v>44047</v>
       </c>
-      <c r="M29" s="4">
-        <v>1</v>
-      </c>
       <c r="N29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="4">
         <v>0</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="17">
+    <row r="30" spans="1:17" ht="17">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -2182,47 +2209,47 @@
       <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>42.959871</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>-123.176224</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="8">
+      <c r="M30" s="8">
         <v>44048</v>
       </c>
-      <c r="M30" s="4">
-        <v>1</v>
-      </c>
       <c r="N30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="4">
         <v>0</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="34">
+    <row r="31" spans="1:17" ht="34">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -2232,47 +2259,47 @@
       <c r="C31" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1600</v>
       </c>
       <c r="H31" s="2">
         <v>1600</v>
       </c>
       <c r="I31" s="2">
+        <v>1600</v>
+      </c>
+      <c r="J31" s="2">
         <v>42.959513000000001</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>-123.176441</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L31" s="8">
+      <c r="M31" s="8">
         <v>44047</v>
       </c>
-      <c r="M31" s="4">
+      <c r="N31" s="4">
         <v>1594</v>
       </c>
-      <c r="N31" s="4">
-        <v>1</v>
-      </c>
       <c r="O31" s="4">
+        <v>1</v>
+      </c>
+      <c r="P31" s="4">
         <v>5</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="17">
+    <row r="32" spans="1:17" ht="17">
       <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
@@ -2282,47 +2309,47 @@
       <c r="C32" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>944</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>735</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>42.958525999999999</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>-123.175899</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L32" s="8">
+      <c r="M32" s="8">
         <v>44048</v>
       </c>
-      <c r="M32" s="4">
+      <c r="N32" s="4">
         <v>2</v>
       </c>
-      <c r="N32" s="4">
+      <c r="O32" s="4">
         <v>942</v>
       </c>
-      <c r="O32" s="4">
-        <v>0</v>
-      </c>
-      <c r="P32" t="s">
+      <c r="P32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:41" ht="17">
+    <row r="33" spans="1:42" ht="17">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
@@ -2332,47 +2359,47 @@
       <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>69</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>150</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>42.957447999999999</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>-123.176174</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L33" s="8">
+      <c r="M33" s="8">
         <v>44048</v>
       </c>
-      <c r="M33" s="4">
+      <c r="N33" s="4">
         <v>2</v>
       </c>
-      <c r="N33" s="4">
+      <c r="O33" s="4">
         <v>68</v>
       </c>
-      <c r="O33" s="4">
-        <v>0</v>
-      </c>
-      <c r="P33" t="s">
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:41" ht="34">
+    <row r="34" spans="1:42" ht="34">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2382,47 +2409,47 @@
       <c r="C34" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="2">
+      <c r="H34" s="2">
         <v>8</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>0.5</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>42.958644999999997</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>-123.17648699999999</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L34" s="8">
+      <c r="M34" s="8">
         <v>44048</v>
       </c>
-      <c r="M34" s="4">
+      <c r="N34" s="4">
         <v>5</v>
       </c>
-      <c r="N34" s="4">
-        <v>0</v>
-      </c>
       <c r="O34" s="4">
-        <v>1</v>
-      </c>
-      <c r="P34" t="s">
+        <v>0</v>
+      </c>
+      <c r="P34" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:41" ht="17">
+    <row r="35" spans="1:42" ht="17">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -2432,47 +2459,47 @@
       <c r="C35" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="2">
+      <c r="H35" s="2">
         <v>36</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>10</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>42.958857999999999</v>
       </c>
-      <c r="J35" s="2">
+      <c r="K35" s="2">
         <v>-123.17660600000001</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L35" s="8">
+      <c r="M35" s="8">
         <v>44048</v>
       </c>
-      <c r="M35" s="4">
+      <c r="N35" s="4">
         <v>36</v>
       </c>
-      <c r="N35" s="4">
-        <v>0</v>
-      </c>
       <c r="O35" s="4">
         <v>0</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
+    <row r="36" spans="1:42">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2482,47 +2509,47 @@
       <c r="C36" t="s">
         <v>17</v>
       </c>
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
       <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
         <v>51</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>39</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>364</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>52.5</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>42.934260000000002</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>-123.03869</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>21</v>
       </c>
-      <c r="L36" s="1">
+      <c r="M36" s="1">
         <v>43292</v>
       </c>
-      <c r="M36" s="4">
-        <v>0</v>
-      </c>
       <c r="N36" s="4">
+        <v>0</v>
+      </c>
+      <c r="O36" s="4">
         <v>364</v>
       </c>
-      <c r="O36" s="4">
-        <v>0</v>
-      </c>
-      <c r="P36" t="s">
+      <c r="P36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:41">
+    <row r="37" spans="1:42">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2532,47 +2559,47 @@
       <c r="C37" t="s">
         <v>23</v>
       </c>
-      <c r="D37" t="s">
-        <v>18</v>
-      </c>
       <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
         <v>51</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>20</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
       <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <v>0.25</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>42.933487</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>-123.03795</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>21</v>
       </c>
-      <c r="L37" s="1">
+      <c r="M37" s="1">
         <v>43292</v>
       </c>
-      <c r="M37" s="4">
-        <v>1</v>
-      </c>
       <c r="N37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" s="4">
         <v>0</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:41" ht="18.75" customHeight="1">
+    <row r="38" spans="1:42" ht="18.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>76</v>
       </c>
@@ -2582,46 +2609,45 @@
       <c r="C38" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>1348</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>1950</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>42.943679000000003</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>-123.011171</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L38" s="8">
+      <c r="M38" s="8">
         <v>44051</v>
       </c>
-      <c r="M38" s="2">
+      <c r="N38" s="2">
         <v>1347</v>
       </c>
-      <c r="N38" s="2">
-        <v>1</v>
-      </c>
       <c r="O38" s="2">
-        <v>0</v>
-      </c>
-      <c r="P38" t="s">
+        <v>1</v>
+      </c>
+      <c r="P38" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="s">
         <v>99</v>
       </c>
-      <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
@@ -2634,8 +2660,8 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="9"/>
-      <c r="AE38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="9"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
@@ -2646,8 +2672,9 @@
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
       <c r="AO38" s="2"/>
-    </row>
-    <row r="39" spans="1:41" ht="16.5" customHeight="1">
+      <c r="AP38" s="2"/>
+    </row>
+    <row r="39" spans="1:42" ht="16.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
@@ -2657,46 +2684,45 @@
       <c r="C39" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>50</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>120</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>42.944516</v>
       </c>
-      <c r="J39" s="2">
+      <c r="K39" s="2">
         <v>-123.00948099999999</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L39" s="8">
+      <c r="M39" s="8">
         <v>44051</v>
       </c>
-      <c r="M39" s="2">
+      <c r="N39" s="2">
         <v>50</v>
       </c>
-      <c r="N39" s="10">
-        <v>0</v>
-      </c>
-      <c r="O39" s="2">
-        <v>0</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="O39" s="10">
+        <v>0</v>
+      </c>
+      <c r="P39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="s">
         <v>99</v>
       </c>
-      <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
@@ -2709,8 +2735,8 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="9"/>
-      <c r="AE39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="9"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
@@ -2721,8 +2747,9 @@
       <c r="AM39" s="2"/>
       <c r="AN39" s="2"/>
       <c r="AO39" s="2"/>
-    </row>
-    <row r="40" spans="1:41">
+      <c r="AP39" s="2"/>
+    </row>
+    <row r="40" spans="1:42">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2732,47 +2759,47 @@
       <c r="C40" t="s">
         <v>17</v>
       </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
       <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
         <v>51</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>20</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>86978</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>931.84</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>42.939444000000002</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>-123.00241</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>21</v>
       </c>
-      <c r="L40" s="1">
+      <c r="M40" s="1">
         <v>43297</v>
       </c>
-      <c r="M40" s="4">
+      <c r="N40" s="4">
         <v>86978</v>
       </c>
-      <c r="N40" s="4">
-        <v>0</v>
-      </c>
       <c r="O40" s="4">
         <v>0</v>
       </c>
-      <c r="P40" t="s">
+      <c r="P40" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:42">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2782,47 +2809,47 @@
       <c r="C41" t="s">
         <v>23</v>
       </c>
-      <c r="D41" t="s">
-        <v>18</v>
-      </c>
       <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
         <v>51</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>20</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>60</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>2.5</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>42.940030999999998</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>-123.003277</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>21</v>
       </c>
-      <c r="L41" s="1">
+      <c r="M41" s="1">
         <v>43297</v>
       </c>
-      <c r="M41" s="4">
+      <c r="N41" s="4">
         <v>60</v>
       </c>
-      <c r="N41" s="4">
-        <v>0</v>
-      </c>
       <c r="O41" s="4">
         <v>0</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:41" ht="22.5" customHeight="1">
+    <row r="42" spans="1:42" ht="22.5" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>80</v>
       </c>
@@ -2832,46 +2859,45 @@
       <c r="C42" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H42" s="2">
         <v>2</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>3</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>42.937823999999999</v>
       </c>
-      <c r="J42" s="2">
+      <c r="K42" s="2">
         <v>-122.993021</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L42" s="8">
+      <c r="M42" s="8">
         <v>44052</v>
       </c>
-      <c r="M42" s="2">
-        <v>1</v>
-      </c>
       <c r="N42" s="2">
         <v>1</v>
       </c>
       <c r="O42" s="2">
-        <v>0</v>
-      </c>
-      <c r="P42" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="s">
         <v>99</v>
       </c>
-      <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
@@ -2884,8 +2910,8 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-      <c r="AD42" s="9"/>
-      <c r="AE42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="9"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
@@ -2896,8 +2922,9 @@
       <c r="AM42" s="2"/>
       <c r="AN42" s="2"/>
       <c r="AO42" s="2"/>
-    </row>
-    <row r="43" spans="1:41" ht="21.75" customHeight="1">
+      <c r="AP42" s="2"/>
+    </row>
+    <row r="43" spans="1:42" ht="21.75" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2907,46 +2934,45 @@
       <c r="C43" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="2">
+      <c r="H43" s="2">
         <v>3114</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>115</v>
       </c>
-      <c r="I43" s="2">
+      <c r="J43" s="2">
         <v>42.937651000000002</v>
       </c>
-      <c r="J43" s="2">
+      <c r="K43" s="2">
         <v>-122.992321</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L43" s="8">
+      <c r="M43" s="8">
         <v>44052</v>
       </c>
-      <c r="M43" s="2">
+      <c r="N43" s="2">
         <v>3114</v>
       </c>
-      <c r="N43" s="2">
-        <v>0</v>
-      </c>
       <c r="O43" s="2">
         <v>0</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="s">
         <v>99</v>
       </c>
-      <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
@@ -2959,8 +2985,8 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
-      <c r="AD43" s="9"/>
-      <c r="AE43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="9"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
@@ -2971,8 +2997,9 @@
       <c r="AM43" s="2"/>
       <c r="AN43" s="2"/>
       <c r="AO43" s="2"/>
-    </row>
-    <row r="44" spans="1:41" ht="20.25" customHeight="1">
+      <c r="AP43" s="2"/>
+    </row>
+    <row r="44" spans="1:42" ht="20.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>82</v>
       </c>
@@ -2982,46 +3009,45 @@
       <c r="C44" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="2">
+      <c r="H44" s="2">
         <v>350</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>25</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>42.937379</v>
       </c>
-      <c r="J44" s="2">
+      <c r="K44" s="2">
         <v>-122.992088</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L44" s="8">
+      <c r="M44" s="8">
         <v>44052</v>
       </c>
-      <c r="M44" s="2">
+      <c r="N44" s="2">
         <v>350</v>
       </c>
-      <c r="N44" s="2">
-        <v>0</v>
-      </c>
       <c r="O44" s="2">
         <v>0</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="s">
         <v>99</v>
       </c>
-      <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
@@ -3034,8 +3060,8 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-      <c r="AD44" s="9"/>
-      <c r="AE44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="9"/>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
@@ -3046,8 +3072,9 @@
       <c r="AM44" s="2"/>
       <c r="AN44" s="2"/>
       <c r="AO44" s="2"/>
-    </row>
-    <row r="45" spans="1:41" ht="17">
+      <c r="AP44" s="2"/>
+    </row>
+    <row r="45" spans="1:42" ht="17">
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
@@ -3057,47 +3084,47 @@
       <c r="C45" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="2">
+      <c r="H45" s="2">
         <v>5</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>10</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>42.936622999999997</v>
       </c>
-      <c r="J45" s="2">
+      <c r="K45" s="2">
         <v>-122.991829</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L45" s="1">
+      <c r="M45" s="1">
         <v>44052</v>
       </c>
-      <c r="M45" s="2">
-        <v>0</v>
-      </c>
       <c r="N45" s="2">
+        <v>0</v>
+      </c>
+      <c r="O45" s="2">
         <v>5</v>
       </c>
-      <c r="O45" s="2">
-        <v>0</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="P45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:41" ht="16.5" customHeight="1">
+    <row r="46" spans="1:42" ht="16.5" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>85</v>
       </c>
@@ -3107,46 +3134,45 @@
       <c r="C46" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="2">
+      <c r="H46" s="2">
         <v>200</v>
       </c>
-      <c r="H46" s="2">
+      <c r="I46" s="2">
         <v>15</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>43.042808999999998</v>
       </c>
-      <c r="J46" s="2">
+      <c r="K46" s="2">
         <v>-122.786841</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L46" s="8">
+      <c r="M46" s="8">
         <v>44051</v>
       </c>
-      <c r="M46" s="2">
+      <c r="N46" s="2">
         <v>200</v>
       </c>
-      <c r="N46" s="2">
-        <v>0</v>
-      </c>
       <c r="O46" s="2">
         <v>0</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="s">
         <v>99</v>
       </c>
-      <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
@@ -3159,8 +3185,8 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
-      <c r="AD46" s="9"/>
-      <c r="AE46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="9"/>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
@@ -3171,8 +3197,9 @@
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
       <c r="AO46" s="2"/>
-    </row>
-    <row r="47" spans="1:41" ht="22.5" customHeight="1">
+      <c r="AP46" s="2"/>
+    </row>
+    <row r="47" spans="1:42" ht="22.5" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>87</v>
       </c>
@@ -3182,46 +3209,45 @@
       <c r="C47" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="2">
+      <c r="H47" s="2">
         <v>2500</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>2400</v>
       </c>
-      <c r="I47" s="2">
+      <c r="J47" s="2">
         <v>43.042180000000002</v>
       </c>
-      <c r="J47" s="2">
+      <c r="K47" s="2">
         <v>-122.78677500000001</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L47" s="8">
+      <c r="M47" s="8">
         <v>44051</v>
       </c>
-      <c r="M47" s="2">
+      <c r="N47" s="2">
         <v>2500</v>
       </c>
-      <c r="N47" s="2">
-        <v>0</v>
-      </c>
       <c r="O47" s="2">
         <v>0</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="s">
         <v>99</v>
       </c>
-      <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
@@ -3234,8 +3260,8 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="9"/>
-      <c r="AE47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="9"/>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
@@ -3246,8 +3272,9 @@
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
       <c r="AO47" s="2"/>
-    </row>
-    <row r="48" spans="1:41">
+      <c r="AP47" s="2"/>
+    </row>
+    <row r="48" spans="1:42">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -3257,47 +3284,47 @@
       <c r="C48" t="s">
         <v>17</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>90</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>91</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>20</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>112</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>43</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>42.89284</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>-123.53474</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="1">
+      <c r="M48" s="1">
         <v>43265</v>
       </c>
-      <c r="M48" s="2">
+      <c r="N48" s="2">
         <v>112</v>
       </c>
-      <c r="N48" s="2">
-        <v>0</v>
-      </c>
       <c r="O48" s="2">
         <v>0</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P48" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -3307,47 +3334,47 @@
       <c r="C49" t="s">
         <v>23</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>90</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>91</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>20</v>
       </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
       <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
         <v>0.25</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>42.891894999999998</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>-123.535178</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>21</v>
       </c>
-      <c r="L49" s="1">
+      <c r="M49" s="1">
         <v>43301</v>
       </c>
-      <c r="M49" s="2">
-        <v>1</v>
-      </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49" s="2">
         <v>0</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P49" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -3357,47 +3384,47 @@
       <c r="C50" t="s">
         <v>23</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>90</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>91</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>20</v>
       </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
       <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>0.25</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>42.889600000000002</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>-123.537688</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>21</v>
       </c>
-      <c r="L50" s="1">
+      <c r="M50" s="1">
         <v>43301</v>
       </c>
-      <c r="M50" s="2">
-        <v>1</v>
-      </c>
       <c r="N50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50" s="2">
         <v>0</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -3407,47 +3434,47 @@
       <c r="C51" t="s">
         <v>23</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>90</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>91</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>39</v>
       </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
       <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
         <v>0.25</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>42.893329999999999</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>-123.53346000000001</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>21</v>
       </c>
-      <c r="L51" s="1">
+      <c r="M51" s="1">
         <v>43361</v>
       </c>
-      <c r="M51" s="2">
-        <v>0</v>
-      </c>
       <c r="N51" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" s="2">
-        <v>0</v>
-      </c>
-      <c r="P51" t="s">
+        <v>1</v>
+      </c>
+      <c r="P51" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -3457,44 +3484,67 @@
       <c r="C52" t="s">
         <v>23</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>90</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>91</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>20</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>2</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>0.5</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>42.865845999999998</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>-123.57890399999999</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>21</v>
       </c>
-      <c r="L52" s="1">
+      <c r="M52" s="1">
         <v>43301</v>
       </c>
-      <c r="M52" s="2">
+      <c r="N52" s="2">
         <v>2</v>
       </c>
-      <c r="N52" s="2">
-        <v>0</v>
-      </c>
       <c r="O52" s="2">
         <v>0</v>
       </c>
-      <c r="P52" t="s">
+      <c r="P52" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="s">
         <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2F523E-3772-A247-94EB-EC12E99B00DA}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>